<commit_message>
Updated template to allow for admission/discharge stats
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Counts" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="24">
   <si>
     <t>2A</t>
   </si>
@@ -87,12 +87,28 @@
   <si>
     <t>Abraj/Others</t>
   </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Trend</t>
+  </si>
+  <si>
+    <t>Out</t>
+  </si>
+  <si>
+    <t>Turnover</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="\+0;\-0;0"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -106,8 +122,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -126,8 +149,14 @@
         <bgColor rgb="FF00FFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -172,11 +201,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -185,17 +277,33 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF57BB8A"/>
+      <color rgb="FFE67C73"/>
+      <color rgb="FF00FFFF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -408,21 +516,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="9" width="7.85546875" customWidth="1"/>
+    <col min="2" max="9" width="6.85546875" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="7.85546875" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.42578125" customWidth="1"/>
+    <col min="14" max="14" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -451,11 +563,23 @@
       <c r="J1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
@@ -490,8 +614,22 @@
         <f t="shared" ref="K2:K8" si="0">SUM(B2:J2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L2" s="5">
+        <v>0</v>
+      </c>
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <f>L2-M2</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="18" t="e">
+        <f>L2/K2</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>10</v>
       </c>
@@ -526,8 +664,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L3" s="5">
+        <v>0</v>
+      </c>
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="19">
+        <f t="shared" ref="N3:N8" si="1">L3-M3</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="18" t="e">
+        <f t="shared" ref="O3:O8" si="2">L3/K3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>11</v>
       </c>
@@ -562,8 +714,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L4" s="5">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
@@ -598,8 +764,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L5" s="5">
+        <v>0</v>
+      </c>
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O5" s="18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>13</v>
       </c>
@@ -634,8 +814,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L6" s="5">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O6" s="18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>14</v>
       </c>
@@ -670,8 +864,22 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L7" s="5">
+        <v>0</v>
+      </c>
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O7" s="18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
@@ -706,54 +914,165 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L8" s="5">
+        <v>0</v>
+      </c>
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O8" s="18" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="7">
-        <f t="shared" ref="B9:K9" si="1">SUM(B2:B8)</f>
+        <f t="shared" ref="B9:K9" si="3">SUM(B2:B8)</f>
         <v>0</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="F9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="H9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="I9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J9" s="7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="16">
+        <f>SUM(L2:L8)</f>
+        <v>0</v>
+      </c>
+      <c r="M9" s="17">
+        <f>SUM(M2:M8)</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="14">
+        <f>SUM(N2:N8)</f>
+        <v>0</v>
+      </c>
+      <c r="O9" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:J8">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:J7">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K2:K8">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B9:J9">
+    <cfRule type="colorScale" priority="11">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L2:L8">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M2:M8">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFE67C73"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FF57BB8A"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N8">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF57BB8A"/>
+        <color rgb="FFFFD666"/>
+        <color rgb="FFE67C73"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -765,43 +1084,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:J7">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFD666"/>
-        <color rgb="FFE67C73"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFD666"/>
-        <color rgb="FFE67C73"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:J9">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFD666"/>
-        <color rgb="FFE67C73"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -812,9 +1096,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -834,220 +1116,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1061,9 +1343,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1083,220 +1363,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1310,9 +1590,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1332,220 +1610,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1559,9 +1837,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1581,220 +1857,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1808,9 +2084,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1830,220 +2104,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2057,9 +2331,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D60"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2079,220 +2351,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2306,9 +2578,7 @@
   </sheetPr>
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2328,220 +2598,220 @@
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="8"/>
+      <c r="D2" s="9"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="9"/>
-      <c r="D3" s="10"/>
+      <c r="A3" s="8"/>
+      <c r="D3" s="9"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="8"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9"/>
-      <c r="D5" s="10"/>
+      <c r="A5" s="8"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="9"/>
-      <c r="D6" s="10"/>
+      <c r="A6" s="8"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="9"/>
-      <c r="D7" s="10"/>
+      <c r="A7" s="8"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="9"/>
-      <c r="D8" s="10"/>
+      <c r="A8" s="8"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="9"/>
-      <c r="D9" s="10"/>
+      <c r="A9" s="8"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="9"/>
-      <c r="D10" s="10"/>
+      <c r="A10" s="8"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="9"/>
-      <c r="D11" s="10"/>
+      <c r="A11" s="8"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9"/>
-      <c r="D12" s="10"/>
+      <c r="A12" s="8"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="9"/>
-      <c r="D13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="9"/>
-      <c r="D14" s="10"/>
+      <c r="A14" s="8"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="9"/>
-      <c r="D15" s="10"/>
+      <c r="A15" s="8"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="9"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="8"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="9"/>
-      <c r="D17" s="10"/>
+      <c r="A17" s="8"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="9"/>
-      <c r="D18" s="10"/>
+      <c r="A18" s="8"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="9"/>
-      <c r="D19" s="10"/>
+      <c r="A19" s="8"/>
+      <c r="D19" s="9"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="9"/>
-      <c r="D20" s="10"/>
+      <c r="A20" s="8"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="9"/>
-      <c r="D21" s="10"/>
+      <c r="A21" s="8"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="9"/>
-      <c r="D22" s="10"/>
+      <c r="A22" s="8"/>
+      <c r="D22" s="9"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="9"/>
-      <c r="D23" s="10"/>
+      <c r="A23" s="8"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="9"/>
-      <c r="D24" s="10"/>
+      <c r="A24" s="8"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="9"/>
-      <c r="D25" s="10"/>
+      <c r="A25" s="8"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="9"/>
-      <c r="D26" s="10"/>
+      <c r="A26" s="8"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="9"/>
-      <c r="D27" s="10"/>
+      <c r="A27" s="8"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="A28" s="8"/>
+      <c r="D28" s="9"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="A29" s="8"/>
+      <c r="D29" s="9"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="9"/>
-      <c r="D30" s="10"/>
+      <c r="A30" s="8"/>
+      <c r="D30" s="9"/>
     </row>
     <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="9"/>
-      <c r="D31" s="10"/>
+      <c r="A31" s="8"/>
+      <c r="D31" s="9"/>
     </row>
     <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="A32" s="8"/>
+      <c r="D32" s="9"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="A33" s="8"/>
+      <c r="D33" s="9"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="9"/>
-      <c r="D34" s="10"/>
+      <c r="A34" s="8"/>
+      <c r="D34" s="9"/>
     </row>
     <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="9"/>
-      <c r="D35" s="10"/>
+      <c r="A35" s="8"/>
+      <c r="D35" s="9"/>
     </row>
     <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="9"/>
-      <c r="D36" s="10"/>
+      <c r="A36" s="8"/>
+      <c r="D36" s="9"/>
     </row>
     <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="9"/>
-      <c r="D37" s="10"/>
+      <c r="A37" s="8"/>
+      <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="9"/>
-      <c r="D38" s="10"/>
+      <c r="A38" s="8"/>
+      <c r="D38" s="9"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="9"/>
-      <c r="D39" s="10"/>
+      <c r="A39" s="8"/>
+      <c r="D39" s="9"/>
     </row>
     <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="9"/>
-      <c r="D40" s="10"/>
+      <c r="A40" s="8"/>
+      <c r="D40" s="9"/>
     </row>
     <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="9"/>
-      <c r="D41" s="10"/>
+      <c r="A41" s="8"/>
+      <c r="D41" s="9"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="9"/>
-      <c r="D42" s="10"/>
+      <c r="A42" s="8"/>
+      <c r="D42" s="9"/>
     </row>
     <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="9"/>
-      <c r="D43" s="10"/>
+      <c r="A43" s="8"/>
+      <c r="D43" s="9"/>
     </row>
     <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D44" s="10"/>
+      <c r="D44" s="9"/>
     </row>
     <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D45" s="10"/>
+      <c r="D45" s="9"/>
     </row>
     <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D46" s="10"/>
+      <c r="D46" s="9"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D47" s="10"/>
+      <c r="D47" s="9"/>
     </row>
     <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D48" s="10"/>
+      <c r="D48" s="9"/>
     </row>
     <row r="49" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D49" s="10"/>
+      <c r="D49" s="9"/>
     </row>
     <row r="50" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D50" s="10"/>
+      <c r="D50" s="9"/>
     </row>
     <row r="51" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D51" s="10"/>
+      <c r="D51" s="9"/>
     </row>
     <row r="52" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D52" s="10"/>
+      <c r="D52" s="9"/>
     </row>
     <row r="53" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D53" s="10"/>
+      <c r="D53" s="9"/>
     </row>
     <row r="54" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D54" s="10"/>
+      <c r="D54" s="9"/>
     </row>
     <row r="55" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D55" s="10"/>
+      <c r="D55" s="9"/>
     </row>
     <row r="56" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D56" s="10"/>
+      <c r="D56" s="9"/>
     </row>
     <row r="57" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D57" s="10"/>
+      <c r="D57" s="9"/>
     </row>
     <row r="58" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D58" s="10"/>
+      <c r="D58" s="9"/>
     </row>
     <row r="59" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D59" s="10"/>
+      <c r="D59" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>